<commit_message>
Update assignment03 grading template
</commit_message>
<xml_diff>
--- a/fall19/assignment02/Grading Template.xlsx
+++ b/fall19/assignment02/Grading Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aavol\Documents\GitHub\aavolo\cmsi186\spring19\assignment02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aavol\Documents\LMU\CMSI 186\Live on Github\f 19\cmsi186\fall19\assignment02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33534D5E-0786-4CA9-9B48-8FFB8BF85D89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D31FA4-1C70-4D61-A455-3AE2AC9769A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" activeTab="2" xr2:uid="{63A3425B-6033-479B-8BF1-9D375DE2499F}"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="29980" windowHeight="19400" activeTab="2" xr2:uid="{63A3425B-6033-479B-8BF1-9D375DE2499F}"/>
   </bookViews>
   <sheets>
     <sheet name="assignment00" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>#</t>
   </si>
@@ -116,9 +116,6 @@
     <t>instance toString works</t>
   </si>
   <si>
-    <t>main for testing exists with ~10 tests in it</t>
-  </si>
-  <si>
     <t>class DiceSet exists</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>getIndividual works</t>
   </si>
   <si>
-    <t>class toString works</t>
-  </si>
-  <si>
     <t>isIdentical works</t>
   </si>
   <si>
@@ -152,9 +146,6 @@
     <t>option 2 roll 1 works</t>
   </si>
   <si>
-    <t>opetion 3 sum works</t>
-  </si>
-  <si>
     <t>option 4 save works</t>
   </si>
   <si>
@@ -183,6 +174,12 @@
   </si>
   <si>
     <t>Hello World uploaded to GitHub</t>
+  </si>
+  <si>
+    <t>class DiceSet</t>
+  </si>
+  <si>
+    <t>option 3 sum works</t>
   </si>
 </sst>
 </file>
@@ -259,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -270,7 +267,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -641,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -652,7 +648,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -663,7 +659,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -674,7 +670,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -887,10 +883,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A814EA-F008-428D-8D17-C9F98DC7D045}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -925,7 +921,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="6">
@@ -940,7 +936,7 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="19"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="6">
         <v>2</v>
       </c>
@@ -953,7 +949,7 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="19"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="6">
         <v>3</v>
       </c>
@@ -966,7 +962,7 @@
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="19"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="6">
         <v>4</v>
       </c>
@@ -979,7 +975,7 @@
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="19"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="6">
         <v>5</v>
       </c>
@@ -992,7 +988,7 @@
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="19"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="6">
         <v>6</v>
       </c>
@@ -1005,53 +1001,53 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="19"/>
-      <c r="C10" s="6">
-        <v>7</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="7">
-        <v>1</v>
-      </c>
-      <c r="F10" s="7"/>
+      <c r="B10" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="11">
+        <v>1</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="20"/>
-      <c r="C11" s="8">
-        <v>8</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>27</v>
+      <c r="B11" s="18"/>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="E11" s="7">
         <v>1</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="6">
+        <v>3</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="13">
-        <v>1</v>
-      </c>
-      <c r="F12" s="13"/>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="19"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13" s="7">
         <v>1</v>
@@ -1059,9 +1055,9 @@
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="19"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>29</v>
@@ -1072,131 +1068,131 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="19"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="6">
+        <v>6</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="18"/>
+      <c r="C16" s="6">
+        <v>7</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="18"/>
+      <c r="C17" s="6">
+        <v>8</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="15">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="18"/>
+      <c r="C19" s="14">
+        <v>2</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="18"/>
+      <c r="C20" s="14">
+        <v>3</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="18"/>
+      <c r="C21" s="14">
         <v>4</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="7">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="19"/>
-      <c r="C16" s="6">
+      <c r="D21" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="18"/>
+      <c r="C22" s="14">
         <v>5</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="7">
-        <v>1</v>
-      </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="19"/>
-      <c r="C17" s="6">
+      <c r="D22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="18"/>
+      <c r="C23" s="14">
         <v>6</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="7">
-        <v>1</v>
-      </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="19"/>
-      <c r="C18" s="6">
+      <c r="D23" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="18"/>
+      <c r="C24" s="14">
         <v>7</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="7">
-        <v>1</v>
-      </c>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="19"/>
-      <c r="C19" s="6">
-        <v>8</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="7">
-        <v>1</v>
-      </c>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="19"/>
-      <c r="C20" s="6">
-        <v>9</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="7">
-        <v>1</v>
-      </c>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="20"/>
-      <c r="C21" s="8">
-        <v>10</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="9">
-        <v>1</v>
-      </c>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="16">
-        <v>1</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="7">
-        <v>1</v>
-      </c>
-      <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="19"/>
-      <c r="C23" s="15">
-        <v>2</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="7">
-        <v>1</v>
-      </c>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="19"/>
-      <c r="C24" s="15">
-        <v>3</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>37</v>
+      <c r="D24" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="E24" s="7">
         <v>1</v>
@@ -1205,119 +1201,67 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="19"/>
-      <c r="C25" s="15">
-        <v>4</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="7">
-        <v>1</v>
-      </c>
-      <c r="F25" s="7"/>
+      <c r="C25" s="17">
+        <v>8</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="8">
+        <v>1</v>
+      </c>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="19"/>
-      <c r="C26" s="15">
-        <v>5</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>39</v>
+      <c r="B26" s="10"/>
+      <c r="C26" s="14">
+        <v>1</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="E26" s="7">
         <v>1</v>
       </c>
-      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="19"/>
-      <c r="C27" s="15">
-        <v>6</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>40</v>
+      <c r="B27" s="10"/>
+      <c r="C27" s="14">
+        <v>2</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="E27" s="7">
         <v>1</v>
       </c>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="19"/>
-      <c r="C28" s="15">
-        <v>7</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="7">
-        <v>1</v>
-      </c>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="20"/>
-      <c r="C29" s="18">
-        <v>8</v>
-      </c>
-      <c r="D29" s="14" t="s">
+    </row>
+    <row r="28" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C28" s="14">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="9">
-        <v>1</v>
-      </c>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="11"/>
-      <c r="C30" s="15">
-        <v>1</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="11"/>
-      <c r="C31" s="15">
+      <c r="E28" s="1">
         <v>2</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C32" s="15">
-        <v>2</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="1">
-        <v>2</v>
-      </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="4:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D33" s="5" t="s">
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E33">
-        <f>SUM(E4:E32)</f>
-        <v>30</v>
+      <c r="E29">
+        <f>SUM(E4:E28)</f>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="B12:B21"/>
-    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="B18:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>